<commit_message>
+Updated with closing applications
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\UiPath\RoboticEnterpriseFramework_ACME project\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shireen.M\Documents\UiPath\Shireen_Capstone_31\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EF616C-9A8B-4011-BD97-27E3AA0C0E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE34B823-C7B7-4B5C-A052-C571CCCC39DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -185,7 +185,7 @@
     <t>AcmeHome</t>
   </si>
   <si>
-    <t>https://acme-test.uipath.com/</t>
+    <t>https://acme-test.uipath.com/home</t>
   </si>
 </sst>
 </file>
@@ -237,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -247,6 +247,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -265,9 +266,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -305,7 +306,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -411,7 +412,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -553,7 +554,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -567,12 +568,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -620,7 +621,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
         <v>42</v>
       </c>
@@ -632,7 +633,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="29">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1648,15 +1649,15 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1693,7 +1694,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1704,7 +1705,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1818,7 +1819,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -1857,7 +1858,7 @@
       <c r="A21" t="s">
         <v>52</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="5" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2840,12 +2841,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.90625" customWidth="1"/>
-    <col min="2" max="2" width="30.08984375" customWidth="1"/>
-    <col min="3" max="3" width="60.36328125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.42578125" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
+Worked on config part
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shireen.M\Documents\UiPath\Shireen_Capstone_31\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shireen.M\Documents\UiPath\Shireen_Capstone_3_A\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE34B823-C7B7-4B5C-A052-C571CCCC39DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97F77D7-CB69-408B-AE48-AA96B5B6C9EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -186,13 +186,28 @@
   </si>
   <si>
     <t>https://acme-test.uipath.com/home</t>
+  </si>
+  <si>
+    <t>AcmeCredentials</t>
+  </si>
+  <si>
+    <t>AcmeLoginCredentials</t>
+  </si>
+  <si>
+    <t>TimeOut</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/work-items/update/</t>
+  </si>
+  <si>
+    <t>WorkUpdate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -214,6 +229,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF464E55"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -247,7 +268,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1649,7 +1670,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1855,16 +1876,37 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>